<commit_message>
feat add shipment type for agent uploading to maintenance
</commit_message>
<xml_diff>
--- a/file-templates/agent-template.xlsx
+++ b/file-templates/agent-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wbmsdiffs\wbms-toplist\file-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D27D1D-2AC7-40E0-8E9A-FD9667102297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D04AC6B1-381C-4665-B240-405D7CF76BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4147CD53-E5A5-4162-B8AD-7F53E566F6FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>CODE</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>SHIPMENT TYPE</t>
+  </si>
+  <si>
+    <t>DOMESTIC</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL - EXPORT</t>
   </si>
 </sst>
 </file>
@@ -511,27 +520,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F5517B-67D6-4E21-92E1-26E6B85ED4D5}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="27.21875" customWidth="1"/>
+    <col min="2" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,63 +548,69 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>6500</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -603,27 +618,30 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>